<commit_message>
Updated the remaining MCH collections
</commit_message>
<xml_diff>
--- a/Historical Papers/Collections/MCH330.xlsx
+++ b/Historical Papers/Collections/MCH330.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="132" yWindow="504" windowWidth="18876" windowHeight="9732"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>identifier</t>
   </si>
@@ -35,29 +38,50 @@
   </si>
   <si>
     <t>file_path</t>
+  </si>
+  <si>
+    <t>MCH330</t>
+  </si>
+  <si>
+    <t>NEWSPAPER CUTTINGS</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>1 Box</t>
+  </si>
+  <si>
+    <t>LOCATION: 33A | GRAP COUNT NUMER: NONE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -65,7 +89,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -75,33 +99,39 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -291,28 +321,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.0"/>
-    <col customWidth="1" min="5" max="5" width="15.13"/>
-    <col customWidth="1" min="6" max="6" width="15.38"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -356,7 +389,26 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>